<commit_message>
Made AdminActivity and now both excels can be imported and added to database
</commit_message>
<xml_diff>
--- a/Idei_Si_Principii/Book1.xlsx
+++ b/Idei_Si_Principii/Book1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian Geanta\Documents\AndroidStudioProjects\SecurityPatrol\Idei_Si_Principii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{F234990E-6BAD-4BC0-8780-A8833D2D4E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35858DF7-0157-4431-A851-2D3E4091E486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,10 +143,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,359 +488,360 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="119.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>100001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
+        <v>100001</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>100001</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2">
+        <v>100001</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
         <v>100002</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100002</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100002</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2">
+        <v>100002</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2">
+        <v>100002</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100002</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2">
         <v>100003</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1">
-        <v>100004</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1">
-        <v>100005</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
-        <v>100006</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2">
+        <v>100003</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1">
-        <v>100007</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100003</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1">
-        <v>100008</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1">
-        <v>100009</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1">
-        <v>100010</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2">
+        <v>100003</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2">
+        <v>100003</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2">
+        <v>100003</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1">
-        <v>100011</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1">
-        <v>100012</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1">
-        <v>100013</v>
-      </c>
-      <c r="E14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="1">
-        <v>100014</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="1">
-        <v>100015</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100016</v>
-      </c>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>